<commit_message>
uploaded By faraz Dasurkar
</commit_message>
<xml_diff>
--- a/excel/testdata.xlsx
+++ b/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,13 +57,13 @@
     <t>1</t>
   </si>
   <si>
+    <t>newTest</t>
+  </si>
+  <si>
+    <t>To check wheter this test is executed</t>
+  </si>
+  <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>newTest</t>
-  </si>
-  <si>
-    <t>To check wheter this test is executed</t>
   </si>
   <si>
     <t>browser</t>
@@ -1066,7 +1066,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1110,21 +1110,21 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -1141,8 +1141,8 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>

</xml_diff>